<commit_message>
change S/X to delta and test.tex
</commit_message>
<xml_diff>
--- a/data/btc_data.xlsx
+++ b/data/btc_data.xlsx
@@ -1374,7 +1374,7 @@
         <v>1.630839866422082</v>
       </c>
       <c r="L24">
-        <v>0.9291159426493237</v>
+        <v>0.929115942649324</v>
       </c>
       <c r="M24">
         <v>1.032916894086315</v>
@@ -1535,7 +1535,7 @@
         <v>-0.6240715846835153</v>
       </c>
       <c r="L28">
-        <v>0.997155786767755</v>
+        <v>0.9971557867677547</v>
       </c>
       <c r="M28">
         <v>1.048799600090004</v>
@@ -1576,7 +1576,7 @@
         <v>-0.3207291791494929</v>
       </c>
       <c r="L29">
-        <v>0.6489750456848878</v>
+        <v>0.648975045684888</v>
       </c>
       <c r="M29">
         <v>1.055297132392146</v>
@@ -2460,7 +2460,7 @@
         <v>-0.3461859732629294</v>
       </c>
       <c r="L51">
-        <v>0.977129153162436</v>
+        <v>0.9771291531624362</v>
       </c>
       <c r="M51">
         <v>1.065469312421961</v>
@@ -3619,7 +3619,7 @@
         <v>0.1188776083834986</v>
       </c>
       <c r="L80">
-        <v>1.667211832136782</v>
+        <v>1.667211832136783</v>
       </c>
       <c r="M80">
         <v>1.087179532182131</v>
@@ -4439,7 +4439,7 @@
         <v>0.041957009351918</v>
       </c>
       <c r="L100">
-        <v>1.429388122418197</v>
+        <v>1.429388122418198</v>
       </c>
       <c r="M100">
         <v>1.081982740857093</v>
@@ -5376,7 +5376,7 @@
         <v>-0.2987234551703462</v>
       </c>
       <c r="L123">
-        <v>0.9634452849956228</v>
+        <v>0.9634452849956225</v>
       </c>
       <c r="M123">
         <v>1.073202199019439</v>
@@ -5619,7 +5619,7 @@
         <v>-0.1065766187786069</v>
       </c>
       <c r="L129">
-        <v>1.06833561145185</v>
+        <v>1.068335611451849</v>
       </c>
       <c r="M129">
         <v>1.051805313308493</v>
@@ -5947,7 +5947,7 @@
         <v>-0.1729720321045052</v>
       </c>
       <c r="L137">
-        <v>1.525894045366554</v>
+        <v>1.525894045366555</v>
       </c>
       <c r="M137">
         <v>1.058396599047589</v>
@@ -6354,7 +6354,7 @@
         <v>-1.23482794500534</v>
       </c>
       <c r="L147">
-        <v>1.221158940871007</v>
+        <v>1.221158940871006</v>
       </c>
       <c r="M147">
         <v>1.052150783406201</v>
@@ -7212,7 +7212,7 @@
         <v>-0.1461169511665018</v>
       </c>
       <c r="L168">
-        <v>1.009688438259681</v>
+        <v>1.00968843825968</v>
       </c>
       <c r="M168">
         <v>1.048745224541275</v>
@@ -7253,7 +7253,7 @@
         <v>-0.1396117576529385</v>
       </c>
       <c r="L169">
-        <v>0.849769624649436</v>
+        <v>0.8497696246494362</v>
       </c>
       <c r="M169">
         <v>1.045527141708408</v>
@@ -7865,7 +7865,7 @@
         <v>1.742358421003322</v>
       </c>
       <c r="L184">
-        <v>0.9621487490738442</v>
+        <v>0.9621487490738443</v>
       </c>
       <c r="M184">
         <v>1.032862100908814</v>
@@ -8474,7 +8474,7 @@
         <v>1.183655634461893</v>
       </c>
       <c r="L199">
-        <v>0.8838818950293855</v>
+        <v>0.8838818950293854</v>
       </c>
       <c r="M199">
         <v>1.012003244522315</v>
@@ -8515,7 +8515,7 @@
         <v>1.15970118320712</v>
       </c>
       <c r="L200">
-        <v>0.9012935574396983</v>
+        <v>0.9012935574396985</v>
       </c>
       <c r="M200">
         <v>1.019869348023324</v>
@@ -8679,7 +8679,7 @@
         <v>1.69868429321838</v>
       </c>
       <c r="L204">
-        <v>0.8602363879298859</v>
+        <v>0.860236387929886</v>
       </c>
       <c r="M204">
         <v>1.006060128798879</v>
@@ -8802,7 +8802,7 @@
         <v>1.70532100756783</v>
       </c>
       <c r="L207">
-        <v>0.9641013904012987</v>
+        <v>0.9641013904012988</v>
       </c>
       <c r="M207">
         <v>1.0030628233354</v>
@@ -9007,7 +9007,7 @@
         <v>0.6950401157623656</v>
       </c>
       <c r="L212">
-        <v>0.8974908868188278</v>
+        <v>0.8974908868188282</v>
       </c>
       <c r="M212">
         <v>1.015115083694141</v>
@@ -9130,7 +9130,7 @@
         <v>0.8266245367247473</v>
       </c>
       <c r="L215">
-        <v>0.9680546517855869</v>
+        <v>0.9680546517855867</v>
       </c>
       <c r="M215">
         <v>1.024831471117265</v>
@@ -9616,7 +9616,7 @@
         <v>0.2672575418267346</v>
       </c>
       <c r="L227">
-        <v>0.9088349655636458</v>
+        <v>0.9088349655636457</v>
       </c>
       <c r="M227">
         <v>1.011649434464328</v>
@@ -9818,7 +9818,7 @@
         <v>0.151747892688212</v>
       </c>
       <c r="L232">
-        <v>0.8114320392942208</v>
+        <v>0.8114320392942207</v>
       </c>
       <c r="M232">
         <v>1.00996463862521</v>
@@ -9900,7 +9900,7 @@
         <v>0.2961567331267596</v>
       </c>
       <c r="L234">
-        <v>0.8788423709901612</v>
+        <v>0.8788423709901613</v>
       </c>
       <c r="M234">
         <v>1.009940597187925</v>
@@ -10102,7 +10102,7 @@
         <v>3.14220646912585</v>
       </c>
       <c r="L239">
-        <v>0.9005938845646287</v>
+        <v>0.9005938845646286</v>
       </c>
       <c r="M239">
         <v>1.03091860380966</v>
@@ -10143,7 +10143,7 @@
         <v>2.528021205004207</v>
       </c>
       <c r="L240">
-        <v>0.9280570602500076</v>
+        <v>0.9280570602500074</v>
       </c>
       <c r="M240">
         <v>1.02683431317428</v>
@@ -10184,7 +10184,7 @@
         <v>2.104517848243974</v>
       </c>
       <c r="L241">
-        <v>0.8077389732314951</v>
+        <v>0.807738973231495</v>
       </c>
       <c r="M241">
         <v>1.029816986103685</v>
@@ -10225,7 +10225,7 @@
         <v>1.750613038399139</v>
       </c>
       <c r="L242">
-        <v>0.9299747641495525</v>
+        <v>0.9299747641495527</v>
       </c>
       <c r="M242">
         <v>1.030106657647533</v>
@@ -10345,7 +10345,7 @@
         <v>1.865451005759533</v>
       </c>
       <c r="L245">
-        <v>0.7517740409329028</v>
+        <v>0.7517740409329027</v>
       </c>
       <c r="M245">
         <v>1.035732194778726</v>
@@ -10509,7 +10509,7 @@
         <v>2.49146414855276</v>
       </c>
       <c r="L249">
-        <v>0.8021333764723116</v>
+        <v>0.8021333764723119</v>
       </c>
       <c r="M249">
         <v>1.017595365408472</v>
@@ -10714,7 +10714,7 @@
         <v>2.523493664718905</v>
       </c>
       <c r="L254">
-        <v>0.776746569748188</v>
+        <v>0.7767465697481882</v>
       </c>
       <c r="M254">
         <v>1.012524075097643</v>
@@ -10919,7 +10919,7 @@
         <v>2.105544522604514</v>
       </c>
       <c r="L259">
-        <v>0.7544078262462345</v>
+        <v>0.7544078262462344</v>
       </c>
       <c r="M259">
         <v>1.025226450638104</v>
@@ -11042,7 +11042,7 @@
         <v>2.10030673681431</v>
       </c>
       <c r="L262">
-        <v>0.6340433186388656</v>
+        <v>0.6340433186388655</v>
       </c>
       <c r="M262">
         <v>1.014279339634409</v>
@@ -11285,7 +11285,7 @@
         <v>1.529355161814965</v>
       </c>
       <c r="L268">
-        <v>0.9005630689560618</v>
+        <v>0.9005630689560616</v>
       </c>
       <c r="M268">
         <v>1.028296535481901</v>
@@ -11367,7 +11367,7 @@
         <v>2.01829675392453</v>
       </c>
       <c r="L270">
-        <v>0.9467220042930884</v>
+        <v>0.9467220042930883</v>
       </c>
       <c r="M270">
         <v>1.019284367074361</v>
@@ -11613,7 +11613,7 @@
         <v>2.74203340713373</v>
       </c>
       <c r="L276">
-        <v>0.9110384752570122</v>
+        <v>0.9110384752570124</v>
       </c>
       <c r="M276">
         <v>1.008267797882913</v>
@@ -11692,7 +11692,7 @@
         <v>2.575451991185614</v>
       </c>
       <c r="L278">
-        <v>0.9120374585080159</v>
+        <v>0.9120374585080158</v>
       </c>
       <c r="M278">
         <v>1.008196607679355</v>
@@ -12017,7 +12017,7 @@
         <v>1.034137037271233</v>
       </c>
       <c r="L286">
-        <v>0.7772245003946756</v>
+        <v>0.7772245003946758</v>
       </c>
       <c r="M286">
         <v>1.010736613616062</v>
@@ -12178,7 +12178,7 @@
         <v>1.510884278307771</v>
       </c>
       <c r="L290">
-        <v>0.8589556976930541</v>
+        <v>0.8589556976930544</v>
       </c>
       <c r="M290">
         <v>1.005657108550768</v>
@@ -12462,7 +12462,7 @@
         <v>0.8812642916626949</v>
       </c>
       <c r="L297">
-        <v>0.8308608149791386</v>
+        <v>0.8308608149791387</v>
       </c>
       <c r="M297">
         <v>1.008456647829106</v>
@@ -12746,7 +12746,7 @@
         <v>1.072092223734881</v>
       </c>
       <c r="L304">
-        <v>0.9980089330284122</v>
+        <v>0.998008933028412</v>
       </c>
       <c r="M304">
         <v>1.008668629244033</v>
@@ -13033,7 +13033,7 @@
         <v>1.181577333422946</v>
       </c>
       <c r="L311">
-        <v>0.9540846826118425</v>
+        <v>0.9540846826118426</v>
       </c>
       <c r="M311">
         <v>1.003954711888591</v>
@@ -13074,7 +13074,7 @@
         <v>-0.4184565460311828</v>
       </c>
       <c r="L312">
-        <v>0.7753219412904719</v>
+        <v>0.7753219412904718</v>
       </c>
       <c r="M312">
         <v>1.010012881401207</v>
@@ -13115,7 +13115,7 @@
         <v>-0.423276137449555</v>
       </c>
       <c r="L313">
-        <v>0.8590504486134907</v>
+        <v>0.8590504486134908</v>
       </c>
       <c r="M313">
         <v>1.007782198961263</v>
@@ -13156,7 +13156,7 @@
         <v>-0.2669110387112087</v>
       </c>
       <c r="L314">
-        <v>0.7823144978910688</v>
+        <v>0.7823144978910685</v>
       </c>
       <c r="M314">
         <v>1.008536305373514</v>
@@ -13197,7 +13197,7 @@
         <v>-0.15026563534834</v>
       </c>
       <c r="L315">
-        <v>0.7886527938944995</v>
+        <v>0.7886527938944994</v>
       </c>
       <c r="M315">
         <v>1.014081867396611</v>
@@ -13320,7 +13320,7 @@
         <v>-0.4137883665441996</v>
       </c>
       <c r="L318">
-        <v>0.8062001874518865</v>
+        <v>0.8062001874518864</v>
       </c>
       <c r="M318">
         <v>1.005586581038564</v>
@@ -13361,7 +13361,7 @@
         <v>-0.04640218142652061</v>
       </c>
       <c r="L319">
-        <v>0.8615351408572197</v>
+        <v>0.8615351408572198</v>
       </c>
       <c r="M319">
         <v>1.006144019940761</v>
@@ -13566,7 +13566,7 @@
         <v>0.8048391931620822</v>
       </c>
       <c r="L324">
-        <v>0.6933618284435155</v>
+        <v>0.6933618284435152</v>
       </c>
       <c r="M324">
         <v>1.012826612559946</v>
@@ -13771,7 +13771,7 @@
         <v>2.082307436795082</v>
       </c>
       <c r="L329">
-        <v>0.8105905755847894</v>
+        <v>0.8105905755847893</v>
       </c>
       <c r="M329">
         <v>1.029927690527371</v>
@@ -13812,7 +13812,7 @@
         <v>2.144518279951354</v>
       </c>
       <c r="L330">
-        <v>0.6746482833060189</v>
+        <v>0.6746482833060187</v>
       </c>
       <c r="M330">
         <v>1.02607939766945</v>
@@ -13853,7 +13853,7 @@
         <v>2.114237500329645</v>
       </c>
       <c r="L331">
-        <v>0.6976604975750317</v>
+        <v>0.6976604975750318</v>
       </c>
       <c r="M331">
         <v>1.020188542697558</v>
@@ -13976,7 +13976,7 @@
         <v>2.319083034798462</v>
       </c>
       <c r="L334">
-        <v>0.7348759271977114</v>
+        <v>0.7348759271977116</v>
       </c>
       <c r="M334">
         <v>1.007876532141188</v>
@@ -14415,7 +14415,7 @@
         <v>2.834886971002653</v>
       </c>
       <c r="L345">
-        <v>0.6809910452713447</v>
+        <v>0.6809910452713448</v>
       </c>
       <c r="M345">
         <v>1.005496042645922</v>
@@ -14699,7 +14699,7 @@
         <v>3.499597401572549</v>
       </c>
       <c r="L352">
-        <v>0.9345104441676049</v>
+        <v>0.9345104441676048</v>
       </c>
       <c r="M352">
         <v>1.010986996660299</v>
@@ -14740,7 +14740,7 @@
         <v>3.421644766285006</v>
       </c>
       <c r="L353">
-        <v>0.7146620001194546</v>
+        <v>0.7146620001194547</v>
       </c>
       <c r="M353">
         <v>1.019498995548959</v>
@@ -14781,7 +14781,7 @@
         <v>3.465805550262973</v>
       </c>
       <c r="L354">
-        <v>0.7086944696004895</v>
+        <v>0.7086944696004897</v>
       </c>
       <c r="M354">
         <v>1.014705863309336</v>
@@ -14945,7 +14945,7 @@
         <v>1.453076323483755</v>
       </c>
       <c r="L358">
-        <v>0.6354992674825619</v>
+        <v>0.6354992674825617</v>
       </c>
       <c r="M358">
         <v>1.011214024244272</v>
@@ -15109,7 +15109,7 @@
         <v>2.223389542008064</v>
       </c>
       <c r="L362">
-        <v>0.8922127628369441</v>
+        <v>0.892212762836944</v>
       </c>
       <c r="M362">
         <v>1.039902691632606</v>
@@ -15513,7 +15513,7 @@
         <v>5.502468634373349</v>
       </c>
       <c r="L372">
-        <v>0.5082270132036125</v>
+        <v>0.5082270132036126</v>
       </c>
       <c r="M372">
         <v>1.028511438484733</v>
@@ -15554,7 +15554,7 @@
         <v>5.502282178952311</v>
       </c>
       <c r="L373">
-        <v>0.5436757497527039</v>
+        <v>0.5436757497527038</v>
       </c>
       <c r="M373">
         <v>1.030689781475715</v>
@@ -15636,7 +15636,7 @@
         <v>7.453805663200608</v>
       </c>
       <c r="L375">
-        <v>0.4996561758346491</v>
+        <v>0.4996561758346492</v>
       </c>
       <c r="M375">
         <v>1.031863119306413</v>
@@ -15677,7 +15677,7 @@
         <v>7.632076660214287</v>
       </c>
       <c r="L376">
-        <v>0.4386632727381166</v>
+        <v>0.4386632727381165</v>
       </c>
       <c r="M376">
         <v>1.033526089324868</v>
@@ -15841,7 +15841,7 @@
         <v>8.441969554355387</v>
       </c>
       <c r="L380">
-        <v>0.3700074114985634</v>
+        <v>0.3700074114985632</v>
       </c>
       <c r="M380">
         <v>1.031371622615059</v>
@@ -15882,7 +15882,7 @@
         <v>8.504102292706486</v>
       </c>
       <c r="L381">
-        <v>0.5600066982626706</v>
+        <v>0.5600066982626707</v>
       </c>
       <c r="M381">
         <v>1.028000607260587</v>
@@ -16485,7 +16485,7 @@
         <v>21.52829887973725</v>
       </c>
       <c r="L396">
-        <v>1.021150434269421</v>
+        <v>1.02115043426942</v>
       </c>
       <c r="M396">
         <v>1.06708606362593</v>
@@ -16687,7 +16687,7 @@
         <v>7.406751869128358</v>
       </c>
       <c r="L401">
-        <v>0.8613248460903569</v>
+        <v>0.8613248460903565</v>
       </c>
       <c r="M401">
         <v>1.049716339006902</v>
@@ -16886,7 +16886,7 @@
         <v>2.884100149092606</v>
       </c>
       <c r="L406">
-        <v>0.9752562810422187</v>
+        <v>0.9752562810422186</v>
       </c>
       <c r="M406">
         <v>1.054549254984246</v>
@@ -16927,7 +16927,7 @@
         <v>2.207533075533347</v>
       </c>
       <c r="L407">
-        <v>1.617051848996045</v>
+        <v>1.617051848996046</v>
       </c>
       <c r="M407">
         <v>1.046128330979007</v>
@@ -17337,7 +17337,7 @@
         <v>0.7368445950736185</v>
       </c>
       <c r="L417">
-        <v>1.356413611616036</v>
+        <v>1.356413611616037</v>
       </c>
       <c r="M417">
         <v>1.056480294709534</v>
@@ -17864,7 +17864,7 @@
         <v>0.01188541993527901</v>
       </c>
       <c r="L430">
-        <v>0.9768622692577406</v>
+        <v>0.9768622692577403</v>
       </c>
       <c r="M430">
         <v>1.034055554078014</v>
@@ -18259,7 +18259,7 @@
         <v>-0.4865619104617092</v>
       </c>
       <c r="L440">
-        <v>0.8594468839436316</v>
+        <v>0.8594468839436317</v>
       </c>
       <c r="M440">
         <v>1.037853519816124</v>

</xml_diff>